<commit_message>
XML és a leírást tartalmazó XLSX file frissítése, felépítés javítása
</commit_message>
<xml_diff>
--- a/MagusTools/SkillDataLegend.xlsx
+++ b/MagusTools/SkillDataLegend.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="101">
   <si>
     <t>difficulty</t>
   </si>
@@ -207,9 +207,6 @@
     <t>level</t>
   </si>
   <si>
-    <t>Ez a képzettség az altípusát a megjelölt képzettségtől veszi a conditions ág függvényében. Ha ilyen nincs, Akkor az adott képzettség neve lesz ennek a képzettségnek az altípusa.</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -259,13 +256,76 @@
   </si>
   <si>
     <t>dependency</t>
+  </si>
+  <si>
+    <t>Az altípust adó képzettség neve</t>
+  </si>
+  <si>
+    <t>&lt;skill&gt;</t>
+  </si>
+  <si>
+    <t>Attributes</t>
+  </si>
+  <si>
+    <t>A képzettség neve</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>&lt;level&gt;</t>
+  </si>
+  <si>
+    <t>Képzettség szintje fokban "type = Levels" esetén</t>
+  </si>
+  <si>
+    <t>Képzettség szintje százalékban "type = Percent" esetén</t>
+  </si>
+  <si>
+    <t>&lt;requirement&gt;</t>
+  </si>
+  <si>
+    <t>lásd. &lt;skill&gt;</t>
+  </si>
+  <si>
+    <t>A követelmény altípusa</t>
+  </si>
+  <si>
+    <t>isdependency</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>A képzettség altípusként ennek a követelménynek az altípusát használja (ha van ilyen)</t>
+  </si>
+  <si>
+    <t>Alapértékként nem örökli egy ráépólő képzettség az alapjának altípusát</t>
+  </si>
+  <si>
+    <t>false (default)</t>
+  </si>
+  <si>
+    <t>&lt;condition&gt;</t>
+  </si>
+  <si>
+    <t>Taglevel</t>
+  </si>
+  <si>
+    <t>&gt;= 3</t>
+  </si>
+  <si>
+    <t>&lt;bonus&gt;</t>
+  </si>
+  <si>
+    <t>&lt;cost&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,6 +385,30 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -334,7 +418,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -480,19 +564,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -545,11 +616,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -573,12 +686,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -586,28 +693,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -629,7 +729,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -638,7 +738,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -647,6 +747,133 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -948,25 +1175,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="15" style="7" customWidth="1"/>
-    <col min="4" max="4" width="84.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="84.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>9</v>
@@ -983,10 +1210,10 @@
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -997,10 +1224,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="15" t="s">
@@ -1011,53 +1238,52 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30" t="s">
+      <c r="A5" s="57"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="27" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="24" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
+      <c r="B7" s="30" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>79</v>
+      <c r="C7" s="54" t="s">
+        <v>78</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="32" t="s">
+      <c r="A8" s="60"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="10" t="s">
         <v>42</v>
@@ -1066,8 +1292,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="39"/>
       <c r="B10" s="8"/>
       <c r="C10" s="10" t="s">
         <v>37</v>
@@ -1077,7 +1303,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="8"/>
       <c r="C11" s="10" t="s">
         <v>44</v>
@@ -1087,7 +1313,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="8"/>
       <c r="C12" s="10" t="s">
         <v>22</v>
@@ -1097,7 +1323,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="8"/>
       <c r="C13" s="10" t="s">
         <v>38</v>
@@ -1107,7 +1333,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="8"/>
       <c r="C14" s="12" t="s">
         <v>47</v>
@@ -1117,7 +1343,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="8"/>
       <c r="C15" s="12" t="s">
         <v>51</v>
@@ -1127,36 +1353,32 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="46"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="30" t="s">
+      <c r="A16" s="39"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="27" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="20"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="38"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="35"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="25" t="s">
+      <c r="A20" s="36"/>
+      <c r="B20" s="23" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="19" t="s">
@@ -1167,20 +1389,20 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="25" t="s">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="23" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="15" t="s">
@@ -1191,8 +1413,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="48"/>
+      <c r="A23" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="43"/>
       <c r="C23" s="10" t="s">
         <v>23</v>
       </c>
@@ -1200,9 +1424,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="49" t="s">
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="24"/>
+      <c r="B24" s="44" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -1213,46 +1437,44 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="49" t="s">
+      <c r="A25" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="50" t="s">
-        <v>71</v>
+      <c r="C25" s="45" t="s">
+        <v>70</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="26" t="s">
+      <c r="A26" s="24"/>
+      <c r="B26" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="49" t="s">
+      <c r="A28" s="24"/>
+      <c r="B28" s="44" t="s">
         <v>17</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -1263,22 +1485,22 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-      <c r="B29" s="49" t="s">
-        <v>73</v>
+      <c r="A29" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>72</v>
       </c>
       <c r="C29" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="49" t="s">
+      <c r="A30" s="24"/>
+      <c r="B30" s="44" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="10" t="s">
@@ -1289,100 +1511,100 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
-      <c r="B31" s="49" t="s">
+      <c r="A31" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="30"/>
+      <c r="B32" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>73</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>74</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
-      <c r="B33" s="49" t="s">
-        <v>73</v>
+      <c r="A33" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>72</v>
       </c>
       <c r="C33" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="11" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" s="49" t="s">
+      <c r="A34" s="28"/>
+      <c r="B34" s="44" t="s">
         <v>17</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
-      <c r="B35" s="49" t="s">
-        <v>73</v>
+      <c r="A35" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="44" t="s">
+        <v>72</v>
       </c>
       <c r="C35" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="11" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" s="49" t="s">
+      <c r="A36" s="28"/>
+      <c r="B36" s="44" t="s">
         <v>17</v>
       </c>
       <c r="C36" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="51"/>
-      <c r="B37" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="10" t="s">
+      <c r="D37" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="52" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="52" t="s">
+      <c r="A38" s="28"/>
+      <c r="B38" s="47" t="s">
         <v>17</v>
       </c>
       <c r="C38" s="10" t="s">
@@ -1393,8 +1615,10 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
-      <c r="B39" s="48"/>
+      <c r="A39" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="43"/>
       <c r="C39" s="10" t="s">
         <v>29</v>
       </c>
@@ -1403,11 +1627,11 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
-      <c r="B40" s="56" t="s">
+      <c r="A40" s="46"/>
+      <c r="B40" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="50" t="s">
+      <c r="C40" s="45" t="s">
         <v>31</v>
       </c>
       <c r="D40" s="11" t="s">
@@ -1415,23 +1639,34 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="B41" s="53"/>
-      <c r="C41" s="54" t="s">
+      <c r="A41" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="48"/>
+      <c r="C41" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="55" t="s">
+      <c r="D41" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
+      <c r="A42" s="42"/>
       <c r="B42" s="21"/>
       <c r="C42" s="9"/>
       <c r="D42" s="22"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="43"/>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1441,13 +1676,540 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" style="63" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="95" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="74" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="64" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="84.42578125" style="74" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="63"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="62" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="115" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="110">
+        <v>1</v>
+      </c>
+      <c r="C2" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="70" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="66" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="71"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="70" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="71"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="71"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="79" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="114" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="71"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="73" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="70" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="66" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="71"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="66" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="71"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="66" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="71"/>
+      <c r="B9" s="96"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="70" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="66" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="71"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="66" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="71"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="66" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="71"/>
+      <c r="B12" s="96"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="71"/>
+      <c r="B13" s="96"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="66" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="71"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="70" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="66" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="116"/>
+      <c r="B15" s="103"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="66" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16" s="75"/>
+      <c r="E16" s="85"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="80" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="110">
+        <v>2</v>
+      </c>
+      <c r="C17" s="90" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="79" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="66" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="116"/>
+      <c r="B18" s="103"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="66" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="93"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="85"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="80" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="110">
+        <v>3</v>
+      </c>
+      <c r="C20" s="90" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="66" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="67"/>
+      <c r="B21" s="96"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="70" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="66" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="67"/>
+      <c r="B22" s="96"/>
+      <c r="C22" s="88"/>
+      <c r="D22" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="67"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="89" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="70" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="66" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="67"/>
+      <c r="B24" s="96"/>
+      <c r="C24" s="89" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="66" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="67"/>
+      <c r="B25" s="96"/>
+      <c r="C25" s="89" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="79" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="66" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="67"/>
+      <c r="B26" s="96"/>
+      <c r="C26" s="90" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="66" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="78"/>
+      <c r="B27" s="103"/>
+      <c r="C27" s="88"/>
+      <c r="D27" s="79" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="66" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="65"/>
+      <c r="B28" s="96"/>
+      <c r="C28" s="93"/>
+      <c r="D28" s="92"/>
+      <c r="E28" s="85"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="80" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="97" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="111" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="66" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="78"/>
+      <c r="B30" s="99"/>
+      <c r="C30" s="104"/>
+      <c r="D30" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="65"/>
+      <c r="B31" s="96"/>
+      <c r="C31" s="93"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="85"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="97">
+        <v>4</v>
+      </c>
+      <c r="C32" s="89" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="66" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="81"/>
+      <c r="B33" s="98"/>
+      <c r="C33" s="90" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="72" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="73" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="105"/>
+      <c r="B34" s="106"/>
+      <c r="C34" s="107"/>
+      <c r="D34" s="105"/>
+      <c r="E34" s="108"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="81" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="98">
+        <v>4</v>
+      </c>
+      <c r="C35" s="88" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="68" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35" s="69" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="101"/>
+      <c r="B36" s="102"/>
+      <c r="C36" s="90" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="72" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="73" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="105"/>
+      <c r="B37" s="106"/>
+      <c r="C37" s="107"/>
+      <c r="D37" s="105"/>
+      <c r="E37" s="108"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" s="98">
+        <v>3</v>
+      </c>
+      <c r="C38" s="87" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="69" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="67"/>
+      <c r="B39" s="98"/>
+      <c r="C39" s="88"/>
+      <c r="D39" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="66" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="67"/>
+      <c r="B40" s="102"/>
+      <c r="C40" s="109" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="77" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" s="73" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="112"/>
+      <c r="B41" s="106"/>
+      <c r="C41" s="107"/>
+      <c r="D41" s="113"/>
+      <c r="E41" s="108"/>
+    </row>
+    <row r="42" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="82" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="100">
+        <v>2</v>
+      </c>
+      <c r="C42" s="91" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="83" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="84" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="76"/>
+      <c r="B43" s="96"/>
+      <c r="C43" s="85"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="85"/>
+    </row>
+    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F81" s="86"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
XML test cases and first draft of FRS
</commit_message>
<xml_diff>
--- a/MagusTools/SkillDataLegend.xlsx
+++ b/MagusTools/SkillDataLegend.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="102">
   <si>
     <t>difficulty</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>&lt;cost&gt;</t>
+  </si>
+  <si>
+    <t>weaponspeed</t>
   </si>
 </sst>
 </file>
@@ -1678,8 +1681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1856,7 +1859,9 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="71"/>
       <c r="B14" s="96"/>
-      <c r="C14" s="94"/>
+      <c r="C14" s="94" t="s">
+        <v>101</v>
+      </c>
       <c r="D14" s="70" t="s">
         <v>51</v>
       </c>

</xml_diff>